<commit_message>
Prbaikn gbest baik done. Next tampilkan
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kuliah\Skripsi\Program\hdpso\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1B49553-F998-48EC-A8CE-1E1D62DF9D1D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1DEDE2B-8C20-4DB7-8656-50A4C99ED939}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -302,8 +302,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-F400]h\.mm\.ss\ AM/PM"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -334,15 +335,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="10">
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="[$-F400]h\.mm\.ss\ AM/PM"/>
     </dxf>
@@ -419,14 +424,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EF8580A4-6CCF-42DA-AFA7-A5285C7EB587}" name="Table5" displayName="Table5" ref="A1:E69" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EF8580A4-6CCF-42DA-AFA7-A5285C7EB587}" name="Table5" displayName="Table5" ref="A1:E69" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="A1:E69" xr:uid="{0E6BFACF-40E7-44F7-A15C-9A57E458C39C}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{65FCFE7B-6B77-4DBE-A45B-4C92406BCA46}" name="No." dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{1ADFF227-93BF-4867-82C5-D5AF24D4858C}" name="Mata Kuliah" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{8C8D9FE0-8267-4665-8054-24D8C4D391A8}" name="SKS" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{F28940BD-1CCF-4494-8913-06C9A53AEDE9}" name="Dosen" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{482DD532-CD36-441D-B26E-C6951383AF59}" name="Kelas" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{65FCFE7B-6B77-4DBE-A45B-4C92406BCA46}" name="No." dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{1ADFF227-93BF-4867-82C5-D5AF24D4858C}" name="Mata Kuliah" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{8C8D9FE0-8267-4665-8054-24D8C4D391A8}" name="SKS" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{F28940BD-1CCF-4494-8913-06C9A53AEDE9}" name="Dosen" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{482DD532-CD36-441D-B26E-C6951383AF59}" name="Kelas" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -448,8 +453,8 @@
   <autoFilter ref="A1:C13" xr:uid="{9CAC7624-DD9C-4606-BC44-FB2F2DE8B0D2}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{B642CF8B-6D2A-462F-AF74-0E5F0579CD25}" name="No."/>
-    <tableColumn id="2" xr3:uid="{B6656088-7644-42FB-A502-597014B0245A}" name="Mulai" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{20900C86-7800-4FB5-9167-0888C1519147}" name="Akhir" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{B6656088-7644-42FB-A502-597014B0245A}" name="Mulai" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{20900C86-7800-4FB5-9167-0888C1519147}" name="Akhir" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -474,7 +479,7 @@
     <tableColumn id="2" xr3:uid="{9C57D199-FC7B-4CC1-A911-0DB32A2B22CF}" name="Limit"/>
     <tableColumn id="3" xr3:uid="{000A58C6-A413-4599-ACF3-3BAB65BC1121}" name="Bloc"/>
     <tableColumn id="4" xr3:uid="{CEBD4721-C897-4FE5-87A4-DA161B63680A}" name="Bglob"/>
-    <tableColumn id="5" xr3:uid="{205AFB75-C810-4A1F-9658-707B446B672B}" name="Brand"/>
+    <tableColumn id="5" xr3:uid="{205AFB75-C810-4A1F-9658-707B446B672B}" name="Brand" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2299,7 +2304,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:E2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2326,19 +2331,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="C2">
+        <v>0.6</v>
+      </c>
+      <c r="D2">
         <v>0.2</v>
       </c>
-      <c r="D2">
-        <v>0.4</v>
-      </c>
-      <c r="E2">
-        <v>0.6</v>
+      <c r="E2" s="3">
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>